<commit_message>
Added rollnumber and email to absentees
</commit_message>
<xml_diff>
--- a/XLS_FILES/absent/absent-Thu Apr 22.xlsx
+++ b/XLS_FILES/absent/absent-Thu Apr 22.xlsx
@@ -11,39 +11,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
   <si>
     <t>Nandita</t>
   </si>
   <si>
+    <t>1811084</t>
+  </si>
+  <si>
     <t>MIP</t>
   </si>
   <si>
     <t>Thu Apr 22</t>
   </si>
   <si>
+    <t>nandita.kadam@somaiya.edu</t>
+  </si>
+  <si>
     <t>Aditya</t>
   </si>
   <si>
+    <t>1811001</t>
+  </si>
+  <si>
     <t>DSIP</t>
   </si>
   <si>
+    <t>aditya.pradhan@somaiya.edu</t>
+  </si>
+  <si>
+    <t>Akshit</t>
+  </si>
+  <si>
+    <t>1811042</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>akshit.gs@somaiya.edu</t>
+  </si>
+  <si>
     <t>Sakshi</t>
   </si>
   <si>
-    <t>AI</t>
-  </si>
-  <si>
-    <t>Akshit</t>
+    <t>1811053</t>
+  </si>
+  <si>
+    <t>sakshi@somaiya.edu</t>
   </si>
 </sst>
 </file>
@@ -420,10 +450,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,49 +469,79 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>